<commit_message>
Start to add mocks to test with metros
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\nik\dev\clockabout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2E414C36-3B51-49CC-9A9C-550DE44D6240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{27535F04-E915-4933-9BFE-971632BB4483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{7ECC6300-DC07-4FC6-BFE6-E9E6FCE2E6B5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Start</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Started at previous pulse</t>
+  </si>
+  <si>
+    <t>Started at previous pulse?</t>
   </si>
 </sst>
 </file>
@@ -2381,7 +2384,7 @@
   <dimension ref="A1:S120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2620,6 +2623,9 @@
       <c r="R10">
         <v>1</v>
       </c>
+      <c r="S10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -2697,6 +2703,9 @@
       <c r="R12">
         <v>2</v>
       </c>
+      <c r="S12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -2776,6 +2785,9 @@
       <c r="R14">
         <v>1</v>
       </c>
+      <c r="S14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -2859,7 +2871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15.093495845794999</v>
       </c>
@@ -2900,7 +2912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15.122391939163</v>
       </c>
@@ -2937,8 +2949,11 @@
       <c r="R18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15.15128493309</v>
       </c>
@@ -2979,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>15.185102939606001</v>
       </c>
@@ -3016,8 +3031,11 @@
       <c r="R20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>15.218080043793</v>
       </c>
@@ -3032,7 +3050,7 @@
         <v>3.2977104186999284E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>15.251245975493999</v>
       </c>
@@ -3047,7 +3065,7 @@
         <v>3.3165931700999352E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>15.284423828125</v>
       </c>
@@ -3062,7 +3080,7 @@
         <v>3.3177852631000704E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>15.317597866058</v>
       </c>
@@ -3077,7 +3095,7 @@
         <v>3.3174037932999667E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>15.350766897202</v>
       </c>
@@ -3092,7 +3110,7 @@
         <v>3.3169031144000272E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>15.399626016617001</v>
       </c>
@@ -3114,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>15.448107004165999</v>
       </c>
@@ -3136,7 +3154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>15.496577978134001</v>
       </c>
@@ -3158,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>15.545068025589</v>
       </c>
@@ -3180,7 +3198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>15.593518972397</v>
       </c>
@@ -3202,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>15.642001867294001</v>
       </c>
@@ -3224,7 +3242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>15.681768894196001</v>
       </c>

</xml_diff>

<commit_message>
Start work on mock _norns.
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\nik\dev\clockabout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{27535F04-E915-4933-9BFE-971632BB4483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4A0D8984-6432-4F1E-AC6C-04573BEC9DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{7ECC6300-DC07-4FC6-BFE6-E9E6FCE2E6B5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Start</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Pulse</t>
   </si>
   <si>
-    <t>Manul workings: 4 pulses per beat, 2 pulses per part, varying swing each beat</t>
-  </si>
-  <si>
     <t>Wanted metro</t>
   </si>
   <si>
@@ -62,6 +59,12 @@
   </si>
   <si>
     <t>Started at previous pulse?</t>
+  </si>
+  <si>
+    <t>Manual workings: 4 pulses per beat, 2 pulses per part, varying swing each beat</t>
+  </si>
+  <si>
+    <t>From init call</t>
   </si>
 </sst>
 </file>
@@ -2384,7 +2387,7 @@
   <dimension ref="A1:S120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2470,7 +2473,7 @@
         <v>8.6390972138000066E-2</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -2524,7 +2527,7 @@
         <v>8</v>
       </c>
       <c r="R7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -2584,7 +2587,10 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -2624,7 +2630,7 @@
         <v>1</v>
       </c>
       <c r="S10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -2704,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="S12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -2786,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="S14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -2868,7 +2874,7 @@
         <v>2</v>
       </c>
       <c r="S16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -2950,7 +2956,7 @@
         <v>1</v>
       </c>
       <c r="S18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -3032,7 +3038,7 @@
         <v>2</v>
       </c>
       <c r="S20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>